<commit_message>
small change to utils -- ready by column
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanatirana/Desktop/delft-visiting/optimize code/scheduling-jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8BDA53-DDB9-D947-9081-137B8A8622AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8930C246-9221-4F43-A631-3F36DC3ECA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="2" xr2:uid="{89AD0465-6C35-FE47-91D1-613292502C79}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="4" xr2:uid="{89AD0465-6C35-FE47-91D1-613292502C79}"/>
   </bookViews>
   <sheets>
     <sheet name="get_fwd_release_delays" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -406,23 +406,23 @@
         <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -432,43 +432,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE041D2-EB11-0840-8B24-BDB78D71FA7C}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>4</v>
-      </c>
-      <c r="B1">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71578EE-A621-4B40-955A-BFE0D3AB3D6B}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
         <v>2</v>
       </c>
-      <c r="C1">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71578EE-A621-4B40-955A-BFE0D3AB3D6B}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>4</v>
       </c>
     </row>
@@ -518,19 +526,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A768FFA-7269-6C46-8592-C35AFE2F5933}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>10</v>
-      </c>
-      <c r="B1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added file for back_propagation -- it is not working
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanatirana/Desktop/delft-visiting/optimize code/scheduling-jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8930C246-9221-4F43-A631-3F36DC3ECA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7C825C-3BFB-8945-A12F-0B35C44DD17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="4" xr2:uid="{89AD0465-6C35-FE47-91D1-613292502C79}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" firstSheet="2" activeTab="7" xr2:uid="{89AD0465-6C35-FE47-91D1-613292502C79}"/>
   </bookViews>
   <sheets>
     <sheet name="get_fwd_release_delays" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="get_fwd_end_local" sheetId="3" r:id="rId3"/>
     <sheet name="get_trans_back" sheetId="4" r:id="rId4"/>
     <sheet name="get_memory_characteristics" sheetId="5" r:id="rId5"/>
+    <sheet name="get_bwd_release_delays" sheetId="6" r:id="rId6"/>
+    <sheet name="get_bwd_proc_compute_node" sheetId="7" r:id="rId7"/>
+    <sheet name="get_bwd_end_local" sheetId="8" r:id="rId8"/>
+    <sheet name="get_grad_trans_back" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -528,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A768FFA-7269-6C46-8592-C35AFE2F5933}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -547,4 +551,137 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B27F04-9FC0-F24B-BEC0-B428E359E494}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE91C5B-2C9C-D444-A97C-AD8E19690B03}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B5DDEE-BB5B-3447-91C0-0A163EE6A841}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB64272B-2AB0-F742-9AB4-95C4E9DB372C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add larger test case
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanatirana/Desktop/delft-visiting/optimize code/scheduling-jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A624ABA2-7C51-F34A-BD7E-6DB6130908DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3148C4-1B3E-2D4D-8CAC-5F0E046B194E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" firstSheet="2" activeTab="6" xr2:uid="{89AD0465-6C35-FE47-91D1-613292502C79}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" firstSheet="2" activeTab="3" xr2:uid="{89AD0465-6C35-FE47-91D1-613292502C79}"/>
   </bookViews>
   <sheets>
     <sheet name="get_fwd_release_delays" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,6 +493,160 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11B2DF9-796E-AF41-8E63-88C35A3E090B}">
   <dimension ref="A1:B3"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A768FFA-7269-6C46-8592-C35AFE2F5933}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B27F04-9FC0-F24B-BEC0-B428E359E494}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE91C5B-2C9C-D444-A97C-AD8E19690B03}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B5DDEE-BB5B-3447-91C0-0A163EE6A841}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB64272B-2AB0-F742-9AB4-95C4E9DB372C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
@@ -526,160 +680,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A768FFA-7269-6C46-8592-C35AFE2F5933}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B27F04-9FC0-F24B-BEC0-B428E359E494}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE91C5B-2C9C-D444-A97C-AD8E19690B03}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B5DDEE-BB5B-3447-91C0-0A163EE6A841}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB64272B-2AB0-F742-9AB4-95C4E9DB372C}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>